<commit_message>
1 new TC committed.
</commit_message>
<xml_diff>
--- a/Data Files/QAtestData.xlsx
+++ b/Data Files/QAtestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayush/Katalon Studio/RplateAndroid/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6808AD10-8DCE-B647-AF84-959495E3C48E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB37E54-5169-3F43-B8FF-D7370F3C3F6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{6B6A885B-1C0A-F140-B3A9-6E9691E67B6C}"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{6B6A885B-1C0A-F140-B3A9-6E9691E67B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Data1</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>ayush.kumar+ft1@revivertest.com</t>
+  </si>
+  <si>
+    <t>ayush.kumar+noplates@revivertest.com</t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B741D4D-2B8B-F04E-95B8-03B83A17A7B0}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,10 +454,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{F189D336-BCA4-884C-91F4-74F91005413A}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{22F59E77-4552-AC43-8703-321833ED79CC}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{D8BB9230-769A-4B40-B0A1-4B1103B8A770}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{75B39527-5010-1341-ADCA-348FD3CF6F88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -462,13 +475,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6664E286-70C0-8040-B0D5-95B8A64F7CA0}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -489,6 +505,14 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -496,6 +520,8 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D5D26E24-D7A0-C64F-A4BC-39713976E9E2}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{F8A5ED93-34BA-FF44-BE58-65244BF02214}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{EE8CF96D-A9B4-9446-AE23-2745CFADA93D}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{17C48282-C226-0548-BF63-55353F7AE8A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>